<commit_message>
imagens desne deletadas e todo código fonte colocado em Python
</commit_message>
<xml_diff>
--- a/Comparacao_Contours57EDG.xlsx
+++ b/Comparacao_Contours57EDG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rodrigo S. Hirama\Documentos\EACH\IC\Classification-of-mammography-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB2D92-6E67-4479-AA86-8B15B413522C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C7F4B9-F3F8-42C4-92C8-C7DEB1930CBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0.05" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -376,6 +376,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,22 +715,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="E25" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="3" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -742,14 +743,15 @@
       <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -763,14 +765,15 @@
         <f>C2/$C$59</f>
         <v>0.49920798261470473</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="8"/>
+      <c r="F2" s="6">
         <v>0.164661</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>4.9461999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -784,14 +787,15 @@
         <f t="shared" ref="D3:D58" si="0">C3/$C$59</f>
         <v>0.38580370453150492</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="8"/>
+      <c r="F3" s="6">
         <v>0.19226399999999999</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>3.9058000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -805,14 +809,15 @@
         <f t="shared" si="0"/>
         <v>0.3739221169119461</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="8"/>
+      <c r="F4" s="6">
         <v>0.108984</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>4.1675999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -826,14 +831,15 @@
         <f t="shared" si="0"/>
         <v>0.49388092875528722</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="8"/>
+      <c r="F5" s="6">
         <v>0.1211</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>3.2752999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -847,14 +853,15 @@
         <f t="shared" si="0"/>
         <v>0.43464251320055169</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="8"/>
+      <c r="F6" s="6">
         <v>0.29388500000000001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>8.4442000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -868,14 +875,15 @@
         <f t="shared" si="0"/>
         <v>0.37856923322421893</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="8"/>
+      <c r="F7" s="6">
         <v>0.172516</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>8.5935999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -889,14 +897,15 @@
         <f t="shared" si="0"/>
         <v>0.49839823779586101</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="8"/>
+      <c r="F8" s="6">
         <v>0.134718</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>6.6604999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -910,14 +919,15 @@
         <f t="shared" si="0"/>
         <v>0.48754805711476695</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="8"/>
+      <c r="F9" s="6">
         <v>0.15690100000000001</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>4.8621999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -931,14 +941,15 @@
         <f t="shared" si="0"/>
         <v>0.49306897676905564</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="8"/>
+      <c r="F10" s="6">
         <v>0.173177</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>9.1689000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -952,14 +963,15 @@
         <f t="shared" si="0"/>
         <v>0.530916926625707</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="8"/>
+      <c r="F11" s="6">
         <v>0.51228200000000002</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0.16439599999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -973,14 +985,15 @@
         <f t="shared" si="0"/>
         <v>0.34096200726586356</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="8"/>
+      <c r="F12" s="6">
         <v>0.22722300000000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>7.9850000000000004E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -994,14 +1007,15 @@
         <f t="shared" si="0"/>
         <v>0.50263436781492998</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="8"/>
+      <c r="F13" s="6">
         <v>0.14644499999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>7.0328000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1015,14 +1029,15 @@
         <f t="shared" si="0"/>
         <v>0.25269541566830089</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="8"/>
+      <c r="F14" s="6">
         <v>0.19375400000000001</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.12637599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1036,14 +1051,15 @@
         <f t="shared" si="0"/>
         <v>0.37761822071902146</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="8"/>
+      <c r="F15" s="6">
         <v>0.117996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>2.4170000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1057,14 +1073,15 @@
         <f t="shared" si="0"/>
         <v>0.50433093206379698</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="8"/>
+      <c r="F16" s="6">
         <v>0.107209</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>4.2299000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1078,14 +1095,15 @@
         <f t="shared" si="0"/>
         <v>0.37801163526930609</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="8"/>
+      <c r="F17" s="6">
         <v>0.15612100000000001</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0.123487</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1099,14 +1117,15 @@
         <f t="shared" si="0"/>
         <v>0.50164063800026848</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="8"/>
+      <c r="F18" s="6">
         <v>0.15762899999999999</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>0.103867</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1120,14 +1139,15 @@
         <f t="shared" si="0"/>
         <v>0.50126370605364801</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="8"/>
+      <c r="F19" s="6">
         <v>0.119112</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>6.5357999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1141,14 +1161,15 @@
         <f t="shared" si="0"/>
         <v>0.50785770833080945</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="8"/>
+      <c r="F20" s="6">
         <v>0.25809199999999999</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>0.184672</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1162,14 +1183,15 @@
         <f t="shared" si="0"/>
         <v>0.3471968031755549</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="8"/>
+      <c r="F21" s="6">
         <v>0.199853</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>0.118254</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1183,14 +1205,15 @@
         <f t="shared" si="0"/>
         <v>0.25741390060694791</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="8"/>
+      <c r="F22" s="6">
         <v>0.14621700000000001</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>6.4579999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1204,14 +1227,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="8"/>
+      <c r="F23" s="6">
         <v>0.84090900000000002</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>0.73023899999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1225,14 +1249,15 @@
         <f t="shared" si="0"/>
         <v>0.49703593425758141</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="8"/>
+      <c r="F24" s="6">
         <v>0.830017</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>0.73467000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1246,14 +1271,15 @@
         <f t="shared" si="0"/>
         <v>0.53415064516214406</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="8"/>
+      <c r="F25" s="6">
         <v>0.28192</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>0.27455299999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1267,14 +1293,15 @@
         <f t="shared" si="0"/>
         <v>0.38055755312598122</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="8"/>
+      <c r="F26" s="6">
         <v>0.623309</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>0.57079999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1288,14 +1315,15 @@
         <f t="shared" si="0"/>
         <v>0.36765247875946472</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="8"/>
+      <c r="F27" s="6">
         <v>0.54652900000000004</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>0.48922399999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1309,14 +1337,15 @@
         <f t="shared" si="0"/>
         <v>0.50180137840064298</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="8"/>
+      <c r="F28" s="6">
         <v>0.87478800000000001</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>0.74290299999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -1330,14 +1359,15 @@
         <f t="shared" si="0"/>
         <v>0.4954604597440842</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="8"/>
+      <c r="F29" s="6">
         <v>0.89290899999999995</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>0.72768200000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1351,14 +1381,15 @@
         <f t="shared" si="0"/>
         <v>0.75133782929281845</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="8"/>
+      <c r="F30" s="6">
         <v>0.986097</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>0.61468599999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1372,14 +1403,15 @@
         <f t="shared" si="0"/>
         <v>0.75122301339854047</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="8"/>
+      <c r="F31" s="6">
         <v>0.95742799999999995</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>0.80099100000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1393,14 +1425,15 @@
         <f t="shared" si="0"/>
         <v>0.36620609901444912</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="8"/>
+      <c r="F32" s="6">
         <v>0.61171399999999998</v>
       </c>
-      <c r="F32" s="2">
+      <c r="G32" s="2">
         <v>0.42631999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -1414,14 +1447,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="8"/>
+      <c r="F33" s="6">
         <v>0.97808499999999998</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>0.73763000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1435,14 +1469,15 @@
         <f t="shared" si="0"/>
         <v>0.7555392160887735</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="8"/>
+      <c r="F34" s="6">
         <v>0.91602399999999995</v>
       </c>
-      <c r="F34" s="2">
+      <c r="G34" s="2">
         <v>0.85323000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1456,14 +1491,15 @@
         <f t="shared" si="0"/>
         <v>0.50745464151449404</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="8"/>
+      <c r="F35" s="6">
         <v>0.86640600000000001</v>
       </c>
-      <c r="F35" s="2">
+      <c r="G35" s="2">
         <v>0.77496100000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1477,14 +1513,15 @@
         <f t="shared" si="0"/>
         <v>0.47663350674258165</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="8"/>
+      <c r="F36" s="6">
         <v>0.75538000000000005</v>
       </c>
-      <c r="F36" s="2">
+      <c r="G36" s="2">
         <v>0.44355899999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1498,14 +1535,15 @@
         <f t="shared" si="0"/>
         <v>0.75632038966535653</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="8"/>
+      <c r="F37" s="6">
         <v>0.93923000000000001</v>
       </c>
-      <c r="F37" s="2">
+      <c r="G37" s="2">
         <v>0.62533499999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1519,14 +1557,15 @@
         <f t="shared" si="0"/>
         <v>0.49701754038128115</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="8"/>
+      <c r="F38" s="6">
         <v>0.13158300000000001</v>
       </c>
-      <c r="F38" s="2">
+      <c r="G38" s="2">
         <v>4.2846000000000002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1540,14 +1579,15 @@
         <f t="shared" si="0"/>
         <v>0.365200784962533</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="8"/>
+      <c r="F39" s="6">
         <v>0.23344500000000001</v>
       </c>
-      <c r="F39" s="2">
+      <c r="G39" s="2">
         <v>8.3718000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1561,14 +1601,15 @@
         <f t="shared" si="0"/>
         <v>0.51746899130180701</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="8"/>
+      <c r="F40" s="6">
         <v>0.17475099999999999</v>
       </c>
-      <c r="F40" s="2">
+      <c r="G40" s="2">
         <v>9.4884999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -1582,14 +1623,15 @@
         <f t="shared" si="0"/>
         <v>0.49506518741561323</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="8"/>
+      <c r="F41" s="6">
         <v>0.15006900000000001</v>
       </c>
-      <c r="F41" s="2">
+      <c r="G41" s="2">
         <v>5.4650999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -1603,14 +1645,15 @@
         <f t="shared" si="0"/>
         <v>0.53897368694532599</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="8"/>
+      <c r="F42" s="6">
         <v>0.80806800000000001</v>
       </c>
-      <c r="F42" s="2">
+      <c r="G42" s="2">
         <v>0.58654899999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -1624,14 +1667,15 @@
         <f t="shared" si="0"/>
         <v>0.50084030869900253</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="8"/>
+      <c r="F43" s="6">
         <v>0.141318</v>
       </c>
-      <c r="F43" s="2">
+      <c r="G43" s="2">
         <v>4.5587999999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -1645,14 +1689,15 @@
         <f t="shared" si="0"/>
         <v>0.5022314237634975</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="8"/>
+      <c r="F44" s="6">
         <v>0.13414699999999999</v>
       </c>
-      <c r="F44" s="2">
+      <c r="G44" s="2">
         <v>0.108722</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -1666,14 +1711,15 @@
         <f t="shared" si="0"/>
         <v>0.48155588086976969</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="8"/>
+      <c r="F45" s="6">
         <v>0.26767800000000003</v>
       </c>
-      <c r="F45" s="2">
+      <c r="G45" s="2">
         <v>9.0305999999999997E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -1687,14 +1733,15 @@
         <f t="shared" si="0"/>
         <v>0.49814755880312028</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="8"/>
+      <c r="F46" s="6">
         <v>0.147177</v>
       </c>
-      <c r="F46" s="2">
+      <c r="G46" s="2">
         <v>5.7561000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -1708,14 +1755,15 @@
         <f t="shared" si="0"/>
         <v>0.50615632304779201</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="8"/>
+      <c r="F47" s="6">
         <v>0.115568</v>
       </c>
-      <c r="F47" s="2">
+      <c r="G47" s="2">
         <v>5.2385000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1729,14 +1777,15 @@
         <f t="shared" si="0"/>
         <v>0.49849118586912317</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="8"/>
+      <c r="F48" s="6">
         <v>0.18184900000000001</v>
       </c>
-      <c r="F48" s="2">
+      <c r="G48" s="2">
         <v>7.0202000000000001E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -1750,14 +1799,15 @@
         <f t="shared" si="0"/>
         <v>0.50020445428083948</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="8"/>
+      <c r="F49" s="6">
         <v>0.150563</v>
       </c>
-      <c r="F49" s="2">
+      <c r="G49" s="2">
         <v>4.1324E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -1771,14 +1821,15 @@
         <f t="shared" si="0"/>
         <v>0.27608440507888088</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="8"/>
+      <c r="F50" s="6">
         <v>0.13585700000000001</v>
       </c>
-      <c r="F50" s="2">
+      <c r="G50" s="2">
         <v>8.9393E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -1792,14 +1843,15 @@
         <f t="shared" si="0"/>
         <v>0.34936640639251726</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="8"/>
+      <c r="F51" s="6">
         <v>0.25971899999999998</v>
       </c>
-      <c r="F51" s="2">
+      <c r="G51" s="2">
         <v>0.100384</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -1813,14 +1865,15 @@
         <f t="shared" si="0"/>
         <v>0.50246168918003797</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="8"/>
+      <c r="F52" s="6">
         <v>0.181312</v>
       </c>
-      <c r="F52" s="2">
+      <c r="G52" s="2">
         <v>0.121827</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -1834,14 +1887,15 @@
         <f t="shared" si="0"/>
         <v>0.36338532727740291</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="8"/>
+      <c r="F53" s="6">
         <v>0.13784099999999999</v>
       </c>
-      <c r="F53" s="2">
+      <c r="G53" s="2">
         <v>7.0684999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -1855,14 +1909,15 @@
         <f t="shared" si="0"/>
         <v>0.3712867072284447</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="8"/>
+      <c r="F54" s="6">
         <v>0.157883</v>
       </c>
-      <c r="F54" s="2">
+      <c r="G54" s="2">
         <v>6.6897999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -1876,14 +1931,15 @@
         <f t="shared" si="0"/>
         <v>0.35962671078540498</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="8"/>
+      <c r="F55" s="6">
         <v>0.436832</v>
       </c>
-      <c r="F55" s="2">
+      <c r="G55" s="2">
         <v>0.14929799999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -1897,14 +1953,15 @@
         <f t="shared" si="0"/>
         <v>0.52859334819110648</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="8"/>
+      <c r="F56" s="6">
         <v>0.28817199999999998</v>
       </c>
-      <c r="F56" s="2">
+      <c r="G56" s="2">
         <v>0.12038699999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -1918,14 +1975,15 @@
         <f t="shared" si="0"/>
         <v>0.75143124261950744</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="8"/>
+      <c r="F57" s="6">
         <v>0.92974900000000005</v>
       </c>
-      <c r="F57" s="2">
+      <c r="G57" s="2">
         <v>0.86445000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>62</v>
       </c>
@@ -1939,19 +1997,20 @@
         <f t="shared" si="0"/>
         <v>0.36374869632736734</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4">
         <v>0.28325800000000001</v>
       </c>
-      <c r="F58" s="5">
+      <c r="G58" s="5">
         <v>0.15459500000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>0</v>
       </c>
@@ -1963,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,12 +2033,12 @@
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="4" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1992,14 +2051,15 @@
       <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2013,14 +2073,15 @@
         <f>C2/$C$59</f>
         <v>0.10579416788755586</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="8"/>
+      <c r="F2" s="6">
         <v>0.164661</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>4.9461999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2034,14 +2095,15 @@
         <f t="shared" ref="D3:D58" si="0">C3/$C$59</f>
         <v>9.9788620813052648E-2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="8"/>
+      <c r="F3" s="6">
         <v>0.19226399999999999</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>3.9058000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2055,14 +2117,15 @@
         <f t="shared" si="0"/>
         <v>7.4702341840764144E-2</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="8"/>
+      <c r="F4" s="6">
         <v>0.108984</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>4.1675999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2076,14 +2139,15 @@
         <f t="shared" si="0"/>
         <v>9.5224527003592754E-2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="8"/>
+      <c r="F5" s="6">
         <v>0.1211</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>3.2752999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2097,14 +2161,15 @@
         <f t="shared" si="0"/>
         <v>9.1641497574865255E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="8"/>
+      <c r="F6" s="6">
         <v>0.29388500000000001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>8.4442000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2118,14 +2183,15 @@
         <f t="shared" si="0"/>
         <v>9.7789749819209251E-2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="8"/>
+      <c r="F7" s="6">
         <v>0.172516</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>8.5935999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2139,14 +2205,15 @@
         <f t="shared" si="0"/>
         <v>7.5612563709246045E-2</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="8"/>
+      <c r="F8" s="6">
         <v>0.134718</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>6.6604999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2160,14 +2227,15 @@
         <f t="shared" si="0"/>
         <v>0.1016588445085367</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="8"/>
+      <c r="F9" s="6">
         <v>0.15690100000000001</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>4.8621999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2181,14 +2249,15 @@
         <f t="shared" si="0"/>
         <v>8.8779066279420255E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="8"/>
+      <c r="F10" s="6">
         <v>0.173177</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>9.1689000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -2202,14 +2271,15 @@
         <f t="shared" si="0"/>
         <v>0.21127571546322116</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="8"/>
+      <c r="F11" s="6">
         <v>0.51228200000000002</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0.16439599999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2223,14 +2293,15 @@
         <f t="shared" si="0"/>
         <v>0.1048509860240411</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="8"/>
+      <c r="F12" s="6">
         <v>0.22722300000000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>7.9850000000000004E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -2244,14 +2315,15 @@
         <f t="shared" si="0"/>
         <v>0.11147647223603011</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="8"/>
+      <c r="F13" s="6">
         <v>0.14644499999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>7.0328000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -2265,14 +2337,15 @@
         <f t="shared" si="0"/>
         <v>0.1042963176932153</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="8"/>
+      <c r="F14" s="6">
         <v>0.19375400000000001</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.12637599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2286,14 +2359,15 @@
         <f t="shared" si="0"/>
         <v>8.182253201044655E-2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="8"/>
+      <c r="F15" s="6">
         <v>0.117996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>2.4170000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -2307,14 +2381,15 @@
         <f t="shared" si="0"/>
         <v>5.5994885540991648E-2</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="8"/>
+      <c r="F16" s="6">
         <v>0.107209</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>4.2299000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -2328,14 +2403,15 @@
         <f t="shared" si="0"/>
         <v>8.0602696411357644E-2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="8"/>
+      <c r="F17" s="6">
         <v>0.15612100000000001</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0.123487</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2349,14 +2425,15 @@
         <f t="shared" si="0"/>
         <v>8.6885692690389052E-2</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="8"/>
+      <c r="F18" s="6">
         <v>0.15762899999999999</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>0.103867</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2370,14 +2447,15 @@
         <f t="shared" si="0"/>
         <v>6.6023161054597407E-2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="8"/>
+      <c r="F19" s="6">
         <v>0.119112</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>6.5357999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2391,14 +2469,15 @@
         <f t="shared" si="0"/>
         <v>0.14259519657641229</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="8"/>
+      <c r="F20" s="6">
         <v>0.25809199999999999</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>0.184672</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2412,14 +2491,15 @@
         <f t="shared" si="0"/>
         <v>0.1120855228332349</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="8"/>
+      <c r="F21" s="6">
         <v>0.199853</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>0.118254</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2433,14 +2513,15 @@
         <f t="shared" si="0"/>
         <v>8.8969026503051052E-2</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="8"/>
+      <c r="F22" s="6">
         <v>0.14621700000000001</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>6.4579999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2454,14 +2535,15 @@
         <f t="shared" si="0"/>
         <v>0.46411431189278018</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="8"/>
+      <c r="F23" s="6">
         <v>0.84090900000000002</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>0.73023899999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -2475,14 +2557,15 @@
         <f t="shared" si="0"/>
         <v>0.57987065107963254</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="8"/>
+      <c r="F24" s="6">
         <v>0.830017</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>0.73467000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2496,14 +2579,15 @@
         <f t="shared" si="0"/>
         <v>0.1518687602903013</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="8"/>
+      <c r="F25" s="6">
         <v>0.28192</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>0.27455299999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2517,14 +2601,15 @@
         <f t="shared" si="0"/>
         <v>0.28690652823190804</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="8"/>
+      <c r="F26" s="6">
         <v>0.623309</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>0.57079999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -2538,14 +2623,15 @@
         <f t="shared" si="0"/>
         <v>0.30659329233923527</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="8"/>
+      <c r="F27" s="6">
         <v>0.54652900000000004</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>0.48922399999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2559,14 +2645,15 @@
         <f t="shared" si="0"/>
         <v>0.717358612706398</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="8"/>
+      <c r="F28" s="6">
         <v>0.87478800000000001</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>0.74290299999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -2580,14 +2667,15 @@
         <f t="shared" si="0"/>
         <v>0.77534710434878396</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="8"/>
+      <c r="F29" s="6">
         <v>0.89290899999999995</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>0.72768200000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -2601,14 +2689,15 @@
         <f t="shared" si="0"/>
         <v>0.85583372306906946</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="8"/>
+      <c r="F30" s="6">
         <v>0.986097</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>0.61468599999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -2622,14 +2711,15 @@
         <f t="shared" si="0"/>
         <v>0.71883770975515449</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="8"/>
+      <c r="F31" s="6">
         <v>0.95742799999999995</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>0.80099100000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2643,14 +2733,15 @@
         <f t="shared" si="0"/>
         <v>0.37514123595966159</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="8"/>
+      <c r="F32" s="6">
         <v>0.61171399999999998</v>
       </c>
-      <c r="F32" s="2">
+      <c r="G32" s="2">
         <v>0.42631999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2664,14 +2755,15 @@
         <f t="shared" si="0"/>
         <v>0.85013709811443749</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="8"/>
+      <c r="F33" s="6">
         <v>0.97808499999999998</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>0.73763000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2685,14 +2777,15 @@
         <f t="shared" si="0"/>
         <v>0.75791886460192048</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="8"/>
+      <c r="F34" s="6">
         <v>0.91602399999999995</v>
       </c>
-      <c r="F34" s="2">
+      <c r="G34" s="2">
         <v>0.85323000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -2706,14 +2799,15 @@
         <f t="shared" si="0"/>
         <v>0.67388975628978098</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="8"/>
+      <c r="F35" s="6">
         <v>0.86640600000000001</v>
       </c>
-      <c r="F35" s="2">
+      <c r="G35" s="2">
         <v>0.77496100000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2727,14 +2821,15 @@
         <f t="shared" si="0"/>
         <v>0.44927841078079944</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="8"/>
+      <c r="F36" s="6">
         <v>0.75538000000000005</v>
       </c>
-      <c r="F36" s="2">
+      <c r="G36" s="2">
         <v>0.44355899999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2748,14 +2843,15 @@
         <f t="shared" si="0"/>
         <v>0.85364271518516999</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="8"/>
+      <c r="F37" s="6">
         <v>0.93923000000000001</v>
       </c>
-      <c r="F37" s="2">
+      <c r="G37" s="2">
         <v>0.62533499999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -2769,14 +2865,15 @@
         <f t="shared" si="0"/>
         <v>6.0019549583664997E-2</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="8"/>
+      <c r="F38" s="6">
         <v>0.13158300000000001</v>
       </c>
-      <c r="F38" s="2">
+      <c r="G38" s="2">
         <v>4.2846000000000002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2790,14 +2887,15 @@
         <f t="shared" si="0"/>
         <v>0.10779304588970536</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="8"/>
+      <c r="F39" s="6">
         <v>0.23344500000000001</v>
       </c>
-      <c r="F39" s="2">
+      <c r="G39" s="2">
         <v>8.3718000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2811,14 +2909,15 @@
         <f t="shared" si="0"/>
         <v>0.11154662224455245</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="8"/>
+      <c r="F40" s="6">
         <v>0.17475099999999999</v>
       </c>
-      <c r="F40" s="2">
+      <c r="G40" s="2">
         <v>9.4884999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -2832,14 +2931,15 @@
         <f t="shared" si="0"/>
         <v>8.9397339651468802E-2</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="8"/>
+      <c r="F41" s="6">
         <v>0.15006900000000001</v>
       </c>
-      <c r="F41" s="2">
+      <c r="G41" s="2">
         <v>5.4650999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2853,14 +2953,15 @@
         <f t="shared" si="0"/>
         <v>0.47301540926696928</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="8"/>
+      <c r="F42" s="6">
         <v>0.80806800000000001</v>
       </c>
-      <c r="F42" s="2">
+      <c r="G42" s="2">
         <v>0.58654899999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -2874,14 +2975,15 @@
         <f t="shared" si="0"/>
         <v>8.0819061720928606E-2</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="8"/>
+      <c r="F43" s="6">
         <v>0.141318</v>
       </c>
-      <c r="F43" s="2">
+      <c r="G43" s="2">
         <v>4.5587999999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -2895,14 +2997,15 @@
         <f t="shared" si="0"/>
         <v>0.10741219890848661</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="8"/>
+      <c r="F44" s="6">
         <v>0.13414699999999999</v>
       </c>
-      <c r="F44" s="2">
+      <c r="G44" s="2">
         <v>0.108722</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -2916,14 +3019,15 @@
         <f t="shared" si="0"/>
         <v>0.13288874140860291</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="8"/>
+      <c r="F45" s="6">
         <v>0.26767800000000003</v>
       </c>
-      <c r="F45" s="2">
+      <c r="G45" s="2">
         <v>9.0305999999999997E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -2937,14 +3041,15 @@
         <f t="shared" si="0"/>
         <v>0.13830299236211294</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="8"/>
+      <c r="F46" s="6">
         <v>0.147177</v>
       </c>
-      <c r="F46" s="2">
+      <c r="G46" s="2">
         <v>5.7561000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -2958,14 +3063,15 @@
         <f t="shared" si="0"/>
         <v>8.8933038649506843E-2</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="8"/>
+      <c r="F47" s="6">
         <v>0.115568</v>
       </c>
-      <c r="F47" s="2">
+      <c r="G47" s="2">
         <v>5.2385000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -2979,14 +3085,15 @@
         <f t="shared" si="0"/>
         <v>6.5204230510150604E-2</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="8"/>
+      <c r="F48" s="6">
         <v>0.18184900000000001</v>
       </c>
-      <c r="F48" s="2">
+      <c r="G48" s="2">
         <v>7.0202000000000001E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -3000,14 +3107,15 @@
         <f t="shared" si="0"/>
         <v>8.8164298655445852E-2</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="8"/>
+      <c r="F49" s="6">
         <v>0.150563</v>
       </c>
-      <c r="F49" s="2">
+      <c r="G49" s="2">
         <v>4.1324E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -3021,14 +3129,15 @@
         <f t="shared" si="0"/>
         <v>0.10643045740437231</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="8"/>
+      <c r="F50" s="6">
         <v>0.13585700000000001</v>
       </c>
-      <c r="F50" s="2">
+      <c r="G50" s="2">
         <v>8.9393E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -3042,14 +3151,15 @@
         <f t="shared" si="0"/>
         <v>0.16250754760706546</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="8"/>
+      <c r="F51" s="6">
         <v>0.25971899999999998</v>
       </c>
-      <c r="F51" s="2">
+      <c r="G51" s="2">
         <v>0.100384</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -3063,14 +3173,15 @@
         <f t="shared" si="0"/>
         <v>0.1356957676061879</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="8"/>
+      <c r="F52" s="6">
         <v>0.181312</v>
       </c>
-      <c r="F52" s="2">
+      <c r="G52" s="2">
         <v>0.121827</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -3084,14 +3195,15 @@
         <f t="shared" si="0"/>
         <v>8.9721866273775597E-2</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="8"/>
+      <c r="F53" s="6">
         <v>0.13784099999999999</v>
       </c>
-      <c r="F53" s="2">
+      <c r="G53" s="2">
         <v>7.0684999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -3105,14 +3217,15 @@
         <f t="shared" si="0"/>
         <v>0.1126089856116074</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="8"/>
+      <c r="F54" s="6">
         <v>0.157883</v>
       </c>
-      <c r="F54" s="2">
+      <c r="G54" s="2">
         <v>6.6897999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -3126,14 +3239,15 @@
         <f t="shared" si="0"/>
         <v>0.25000865044386106</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="8"/>
+      <c r="F55" s="6">
         <v>0.436832</v>
       </c>
-      <c r="F55" s="2">
+      <c r="G55" s="2">
         <v>0.14929799999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -3147,14 +3261,15 @@
         <f t="shared" si="0"/>
         <v>0.1125788010153128</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="8"/>
+      <c r="F56" s="6">
         <v>0.28817199999999998</v>
       </c>
-      <c r="F56" s="2">
+      <c r="G56" s="2">
         <v>0.12038699999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -3168,14 +3283,15 @@
         <f t="shared" si="0"/>
         <v>0.69556966559058153</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="8"/>
+      <c r="F57" s="6">
         <v>0.92974900000000005</v>
       </c>
-      <c r="F57" s="2">
+      <c r="G57" s="2">
         <v>0.86445000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>62</v>
       </c>
@@ -3189,19 +3305,20 @@
         <f t="shared" si="0"/>
         <v>0.16182249330820681</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4">
         <v>0.28325800000000001</v>
       </c>
-      <c r="F58" s="5">
+      <c r="G58" s="5">
         <v>0.15459500000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>0</v>
       </c>
@@ -3213,22 +3330,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="3" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3241,14 +3358,15 @@
       <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3262,14 +3380,15 @@
         <f>C2/$C$59</f>
         <v>9.5168586683935297E-2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="8"/>
+      <c r="F2" s="6">
         <v>0.164661</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>4.9461999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3283,14 +3402,15 @@
         <f t="shared" ref="D3:D58" si="0">C3/$C$59</f>
         <v>7.1566718081140707E-2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="8"/>
+      <c r="F3" s="6">
         <v>0.19226399999999999</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>3.9058000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -3304,14 +3424,15 @@
         <f t="shared" si="0"/>
         <v>9.0002849562974899E-2</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="8"/>
+      <c r="F4" s="6">
         <v>0.108984</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>4.1675999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3325,14 +3446,15 @@
         <f t="shared" si="0"/>
         <v>4.1258151001408588E-2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="8"/>
+      <c r="F5" s="6">
         <v>0.1211</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>3.2752999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3346,14 +3468,15 @@
         <f t="shared" si="0"/>
         <v>0.14455622121549949</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="8"/>
+      <c r="F6" s="6">
         <v>0.29388500000000001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>8.4442000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3367,14 +3490,15 @@
         <f t="shared" si="0"/>
         <v>0.13069225463536874</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="8"/>
+      <c r="F7" s="6">
         <v>0.172516</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>8.5935999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -3388,14 +3512,15 @@
         <f t="shared" si="0"/>
         <v>0.11529407427808415</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="8"/>
+      <c r="F8" s="6">
         <v>0.134718</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>6.6604999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -3409,14 +3534,15 @@
         <f t="shared" si="0"/>
         <v>0.10087493507676321</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="8"/>
+      <c r="F9" s="6">
         <v>0.15690100000000001</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>4.8621999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -3430,14 +3556,15 @@
         <f t="shared" si="0"/>
         <v>0.12518848275163</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="8"/>
+      <c r="F10" s="6">
         <v>0.173177</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>9.1689000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -3451,14 +3578,15 @@
         <f t="shared" si="0"/>
         <v>0.12377460946049346</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="8"/>
+      <c r="F11" s="6">
         <v>0.51228200000000002</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0.16439599999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -3472,14 +3600,15 @@
         <f t="shared" si="0"/>
         <v>6.7677193458248006E-2</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="8"/>
+      <c r="F12" s="6">
         <v>0.22722300000000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>7.9850000000000004E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -3493,14 +3622,15 @@
         <f t="shared" si="0"/>
         <v>0.13246641926125094</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="8"/>
+      <c r="F13" s="6">
         <v>0.14644499999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>7.0328000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -3514,14 +3644,15 @@
         <f t="shared" si="0"/>
         <v>0.1242113798522289</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="8"/>
+      <c r="F14" s="6">
         <v>0.19375400000000001</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.12637599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3535,14 +3666,15 @@
         <f t="shared" si="0"/>
         <v>3.2699774454645059E-2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="8"/>
+      <c r="F15" s="6">
         <v>0.117996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>2.4170000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -3556,14 +3688,15 @@
         <f t="shared" si="0"/>
         <v>0.1033291811133481</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="8"/>
+      <c r="F16" s="6">
         <v>0.107209</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>4.2299000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -3577,14 +3710,15 @@
         <f t="shared" si="0"/>
         <v>0.12690493091851526</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="8"/>
+      <c r="F17" s="6">
         <v>0.15612100000000001</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0.123487</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -3598,14 +3732,15 @@
         <f t="shared" si="0"/>
         <v>0.12946424461395145</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="8"/>
+      <c r="F18" s="6">
         <v>0.15762899999999999</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>0.103867</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -3619,14 +3754,15 @@
         <f t="shared" si="0"/>
         <v>0.13238809991615544</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="8"/>
+      <c r="F19" s="6">
         <v>0.119112</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>6.5357999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -3640,14 +3776,15 @@
         <f t="shared" si="0"/>
         <v>0.14644660940672621</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="8"/>
+      <c r="F20" s="6">
         <v>0.25809199999999999</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>0.184672</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -3661,14 +3798,15 @@
         <f t="shared" si="0"/>
         <v>0.13344588414640626</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="8"/>
+      <c r="F21" s="6">
         <v>0.199853</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>0.118254</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -3682,14 +3820,15 @@
         <f t="shared" si="0"/>
         <v>0.13228356819206119</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="8"/>
+      <c r="F22" s="6">
         <v>0.14621700000000001</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>6.4579999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -3703,14 +3842,15 @@
         <f t="shared" si="0"/>
         <v>0.52776400266490697</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="8"/>
+      <c r="F23" s="6">
         <v>0.84090900000000002</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>0.73023899999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -3724,14 +3864,15 @@
         <f t="shared" si="0"/>
         <v>0.27798867346871126</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="8"/>
+      <c r="F24" s="6">
         <v>0.830017</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>0.73467000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -3745,14 +3886,15 @@
         <f t="shared" si="0"/>
         <v>0.15952272300108589</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="8"/>
+      <c r="F25" s="6">
         <v>0.28192</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>0.27455299999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3766,14 +3908,15 @@
         <f t="shared" si="0"/>
         <v>0.21228634576224134</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="8"/>
+      <c r="F26" s="6">
         <v>0.623309</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>0.57079999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -3787,14 +3930,15 @@
         <f t="shared" si="0"/>
         <v>0.22465124452480359</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="8"/>
+      <c r="F27" s="6">
         <v>0.54652900000000004</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>0.48922399999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -3808,14 +3952,15 @@
         <f t="shared" si="0"/>
         <v>0.31036025282212126</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="8"/>
+      <c r="F28" s="6">
         <v>0.87478800000000001</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>0.74290299999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -3829,14 +3974,15 @@
         <f t="shared" si="0"/>
         <v>0.25215488995740104</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="8"/>
+      <c r="F29" s="6">
         <v>0.89290899999999995</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>0.72768200000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -3850,14 +3996,15 @@
         <f t="shared" si="0"/>
         <v>0.77631726768256648</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="8"/>
+      <c r="F30" s="6">
         <v>0.986097</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>0.61468599999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -3871,14 +4018,15 @@
         <f t="shared" si="0"/>
         <v>0.66730195196733499</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="8"/>
+      <c r="F31" s="6">
         <v>0.95742799999999995</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>0.80099100000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -3892,14 +4040,15 @@
         <f t="shared" si="0"/>
         <v>0.14399135599896176</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="8"/>
+      <c r="F32" s="6">
         <v>0.61171399999999998</v>
       </c>
-      <c r="F32" s="2">
+      <c r="G32" s="2">
         <v>0.42631999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -3913,14 +4062,15 @@
         <f t="shared" si="0"/>
         <v>0.66952531454200848</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="8"/>
+      <c r="F33" s="6">
         <v>0.97808499999999998</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>0.73763000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -3934,14 +4084,15 @@
         <f t="shared" si="0"/>
         <v>0.40600188687893674</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="8"/>
+      <c r="F34" s="6">
         <v>0.91602399999999995</v>
       </c>
-      <c r="F34" s="2">
+      <c r="G34" s="2">
         <v>0.85323000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -3955,14 +4106,15 @@
         <f t="shared" si="0"/>
         <v>0.22372901619736216</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="8"/>
+      <c r="F35" s="6">
         <v>0.86640600000000001</v>
       </c>
-      <c r="F35" s="2">
+      <c r="G35" s="2">
         <v>0.77496100000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -3976,14 +4128,15 @@
         <f t="shared" si="0"/>
         <v>0.19981295714103475</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="8"/>
+      <c r="F36" s="6">
         <v>0.75538000000000005</v>
       </c>
-      <c r="F36" s="2">
+      <c r="G36" s="2">
         <v>0.44355899999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -3997,14 +4150,15 @@
         <f t="shared" si="0"/>
         <v>0.37756479336297999</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="8"/>
+      <c r="F37" s="6">
         <v>0.93923000000000001</v>
       </c>
-      <c r="F37" s="2">
+      <c r="G37" s="2">
         <v>0.62533499999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -4018,14 +4172,15 @@
         <f t="shared" si="0"/>
         <v>8.8796447848166996E-2</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="8"/>
+      <c r="F38" s="6">
         <v>0.13158300000000001</v>
       </c>
-      <c r="F38" s="2">
+      <c r="G38" s="2">
         <v>4.2846000000000002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -4039,14 +4194,15 @@
         <f t="shared" si="0"/>
         <v>4.1796488200281597E-2</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="8"/>
+      <c r="F39" s="6">
         <v>0.23344500000000001</v>
       </c>
-      <c r="F39" s="2">
+      <c r="G39" s="2">
         <v>8.3718000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -4060,14 +4216,15 @@
         <f t="shared" si="0"/>
         <v>9.3122784393348201E-2</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="8"/>
+      <c r="F40" s="6">
         <v>0.17475099999999999</v>
       </c>
-      <c r="F40" s="2">
+      <c r="G40" s="2">
         <v>9.4884999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -4081,14 +4238,15 @@
         <f t="shared" si="0"/>
         <v>9.1335714081438299E-2</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="8"/>
+      <c r="F41" s="6">
         <v>0.15006900000000001</v>
       </c>
-      <c r="F41" s="2">
+      <c r="G41" s="2">
         <v>5.4650999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -4102,14 +4260,15 @@
         <f t="shared" si="0"/>
         <v>0.31854471927137062</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="8"/>
+      <c r="F42" s="6">
         <v>0.80806800000000001</v>
       </c>
-      <c r="F42" s="2">
+      <c r="G42" s="2">
         <v>0.58654899999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -4123,14 +4282,15 @@
         <f t="shared" si="0"/>
         <v>7.5125547019995645E-2</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="8"/>
+      <c r="F43" s="6">
         <v>0.141318</v>
       </c>
-      <c r="F43" s="2">
+      <c r="G43" s="2">
         <v>4.5587999999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -4144,14 +4304,15 @@
         <f t="shared" si="0"/>
         <v>0.13394213850671771</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="8"/>
+      <c r="F44" s="6">
         <v>0.13414699999999999</v>
       </c>
-      <c r="F44" s="2">
+      <c r="G44" s="2">
         <v>0.108722</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -4165,14 +4326,15 @@
         <f t="shared" si="0"/>
         <v>8.7964994159753396E-2</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="8"/>
+      <c r="F45" s="6">
         <v>0.26767800000000003</v>
       </c>
-      <c r="F45" s="2">
+      <c r="G45" s="2">
         <v>9.0305999999999997E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -4186,14 +4348,15 @@
         <f t="shared" si="0"/>
         <v>8.4699427570616645E-2</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="8"/>
+      <c r="F46" s="6">
         <v>0.147177</v>
       </c>
-      <c r="F46" s="2">
+      <c r="G46" s="2">
         <v>5.7561000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -4207,14 +4370,15 @@
         <f t="shared" si="0"/>
         <v>0.12535281674065751</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="8"/>
+      <c r="F47" s="6">
         <v>0.115568</v>
       </c>
-      <c r="F47" s="2">
+      <c r="G47" s="2">
         <v>5.2385000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -4228,14 +4392,15 @@
         <f t="shared" si="0"/>
         <v>0.10056559870008315</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="8"/>
+      <c r="F48" s="6">
         <v>0.18184900000000001</v>
       </c>
-      <c r="F48" s="2">
+      <c r="G48" s="2">
         <v>7.0202000000000001E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -4249,14 +4414,15 @@
         <f t="shared" si="0"/>
         <v>6.2301638259015503E-2</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="8"/>
+      <c r="F49" s="6">
         <v>0.150563</v>
       </c>
-      <c r="F49" s="2">
+      <c r="G49" s="2">
         <v>4.1324E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -4270,14 +4436,15 @@
         <f t="shared" si="0"/>
         <v>0.11568516498187049</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="8"/>
+      <c r="F50" s="6">
         <v>0.13585700000000001</v>
       </c>
-      <c r="F50" s="2">
+      <c r="G50" s="2">
         <v>8.9393E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -4291,14 +4458,15 @@
         <f t="shared" si="0"/>
         <v>8.6431644214981854E-2</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="8"/>
+      <c r="F51" s="6">
         <v>0.25971899999999998</v>
       </c>
-      <c r="F51" s="2">
+      <c r="G51" s="2">
         <v>0.100384</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -4312,14 +4480,15 @@
         <f t="shared" si="0"/>
         <v>8.9959752964325096E-2</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="8"/>
+      <c r="F52" s="6">
         <v>0.181312</v>
       </c>
-      <c r="F52" s="2">
+      <c r="G52" s="2">
         <v>0.121827</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -4333,14 +4502,15 @@
         <f t="shared" si="0"/>
         <v>0.12161445116079625</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="8"/>
+      <c r="F53" s="6">
         <v>0.13784099999999999</v>
       </c>
-      <c r="F53" s="2">
+      <c r="G53" s="2">
         <v>7.0684999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -4354,14 +4524,15 @@
         <f t="shared" si="0"/>
         <v>7.59557014483698E-2</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="8"/>
+      <c r="F54" s="6">
         <v>0.157883</v>
       </c>
-      <c r="F54" s="2">
+      <c r="G54" s="2">
         <v>6.6897999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -4375,14 +4546,15 @@
         <f t="shared" si="0"/>
         <v>6.1624107129325249E-2</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="8"/>
+      <c r="F55" s="6">
         <v>0.436832</v>
       </c>
-      <c r="F55" s="2">
+      <c r="G55" s="2">
         <v>0.14929799999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -4396,14 +4568,15 @@
         <f t="shared" si="0"/>
         <v>0.11998236874062206</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="8"/>
+      <c r="F56" s="6">
         <v>0.28817199999999998</v>
       </c>
-      <c r="F56" s="2">
+      <c r="G56" s="2">
         <v>0.12038699999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -4417,14 +4590,15 @@
         <f t="shared" si="0"/>
         <v>0.58866984516635545</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="8"/>
+      <c r="F57" s="6">
         <v>0.92974900000000005</v>
       </c>
-      <c r="F57" s="2">
+      <c r="G57" s="2">
         <v>0.86445000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>62</v>
       </c>
@@ -4438,19 +4612,20 @@
         <f t="shared" si="0"/>
         <v>7.6947625733306144E-2</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4">
         <v>0.28325800000000001</v>
       </c>
-      <c r="F58" s="5">
+      <c r="G58" s="5">
         <v>0.15459500000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>0</v>
       </c>

</xml_diff>